<commit_message>
added assays using ARCitect
</commit_message>
<xml_diff>
--- a/studies/language-usage/isa.study.xlsx
+++ b/studies/language-usage/isa.study.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>STUDY</t>
   </si>
@@ -169,9 +169,15 @@
     <t>Study Person Last Name</t>
   </si>
   <si>
+    <t>Krumsieck</t>
+  </si>
+  <si>
     <t>Study Person First Name</t>
   </si>
   <si>
+    <t>Jens</t>
+  </si>
+  <si>
     <t>Study Person Mid Initials</t>
   </si>
   <si>
@@ -190,6 +196,9 @@
     <t>Study Person Affiliation</t>
   </si>
   <si>
+    <t>Johann Heinrich von Thünen-Institut, Zentrum für Informationsmanagement;Technische Universität Braunschweig, Institut für Anorganische und Analytische Chemie</t>
+  </si>
+  <si>
     <t>Study Person Roles</t>
   </si>
   <si>
@@ -197,6 +206,12 @@
   </si>
   <si>
     <t>Study Person Roles Term Source REF</t>
+  </si>
+  <si>
+    <t>Comment[ORCID]</t>
+  </si>
+  <si>
+    <t>0000-0001-6242-5846</t>
   </si>
 </sst>
 </file>
@@ -548,7 +563,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B61"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -802,59 +817,76 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="B51" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>60</v>
+      </c>
+      <c r="B57" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B61" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>